<commit_message>
dry weights F2 and F2 update
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Physiology/Phys_data_tracker.xlsx
+++ b/RAnalysis/Data/Physiology/Phys_data_tracker.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.gurr\Documents\Github_repositories\Airradians_multigen_OA\RAnalysis\Data\Physiology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Github_repositories\Airradians_multigen_OA\RAnalysis\Data\Physiology\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0261106-2214-4944-BA14-576D268D25D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1176" yWindow="0" windowWidth="25200" windowHeight="11988"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -135,12 +136,15 @@
   </si>
   <si>
     <t>Depurvated (yes / no)</t>
+  </si>
+  <si>
+    <t>~'58 mL small static chambers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -256,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -311,6 +315,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -592,29 +599,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="1" customWidth="1"/>
     <col min="4" max="4" width="22" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="19.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="37.21875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="25.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6328125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="19.54296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="37.1796875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -637,7 +644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="15" t="s">
@@ -666,7 +673,7 @@
       </c>
       <c r="K2" s="15"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44453</v>
       </c>
@@ -701,7 +708,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44469</v>
       </c>
@@ -736,7 +743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44495</v>
       </c>
@@ -771,7 +778,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44495</v>
       </c>
@@ -806,7 +813,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44594</v>
       </c>
@@ -839,7 +846,7 @@
       </c>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44621</v>
       </c>
@@ -872,7 +879,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44826</v>
       </c>
@@ -905,7 +912,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>44860</v>
       </c>
@@ -938,7 +945,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="9"/>
@@ -954,7 +961,7 @@
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>44671</v>
       </c>
@@ -989,7 +996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44673</v>
       </c>
@@ -1024,7 +1031,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>44797</v>
       </c>
@@ -1057,7 +1064,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44802</v>
       </c>
@@ -1092,7 +1099,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>44803</v>
       </c>
@@ -1125,7 +1132,7 @@
       </c>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>44826</v>
       </c>
@@ -1158,30 +1165,62 @@
       </c>
       <c r="K17" s="8"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>44881</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:I15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I15">
     <sortCondition ref="A2:A15"/>
     <sortCondition ref="B2:B15"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A22" r:id="rId1" location="gid=1870016393" display="https://docs.google.com/spreadsheets/d/1o02P1kmXS3jQ48BZF9ssCqJM2U9f5KeQRMVTCl-cDks/edit - gid=1870016393"/>
+    <hyperlink ref="A22" r:id="rId1" location="gid=1870016393" display="https://docs.google.com/spreadsheets/d/1o02P1kmXS3jQ48BZF9ssCqJM2U9f5KeQRMVTCl-cDks/edit - gid=1870016393" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>